<commit_message>
Some refactoring to reduce IL size and allow up to 255 degrees of liberty in Student distribution
</commit_message>
<xml_diff>
--- a/Student.xlsx
+++ b/Student.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mrener/Projects/Repzilon.Libraries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E1C26AC-2A39-F742-BD1C-C75A87118D87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5B3E03-F0F3-6549-94F8-90A8AF5BDFCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="-7500" windowWidth="38400" windowHeight="23500" xr2:uid="{A7CD8C95-85D1-1E4C-B771-A6F8EF459DDC}"/>
+    <workbookView xWindow="51400" yWindow="-7500" windowWidth="12600" windowHeight="23500" activeTab="2" xr2:uid="{A7CD8C95-85D1-1E4C-B771-A6F8EF459DDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Graphique1" sheetId="2" r:id="rId1"/>
     <sheet name="Feuil1" sheetId="1" r:id="rId2"/>
+    <sheet name="Code size" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,27 +38,111 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
   <si>
     <t>x</t>
   </si>
   <si>
     <t>k</t>
   </si>
+  <si>
+    <t>Méthode</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>.cctor()</t>
+  </si>
+  <si>
+    <t>AddGammaHalves</t>
+  </si>
+  <si>
+    <t>AddGammaIntegers</t>
+  </si>
+  <si>
+    <t>BigProduct</t>
+  </si>
+  <si>
+    <t>GammaRatio</t>
+  </si>
+  <si>
+    <t>Normal(r8, r8, r8, bool)</t>
+  </si>
+  <si>
+    <t>Normal(r8, bool)</t>
+  </si>
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>ProductOfIntegers</t>
+  </si>
+  <si>
+    <t>RemoveIdenticalFactors</t>
+  </si>
+  <si>
+    <t>SplitDividableBy</t>
+  </si>
+  <si>
+    <t>SplitDividableByThree</t>
+  </si>
+  <si>
+    <t>SplitEvenNumbers</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Itération 1</t>
+  </si>
+  <si>
+    <t>Itération 2</t>
+  </si>
+  <si>
+    <t>RemoveDividableFactors</t>
+  </si>
+  <si>
+    <t>RemoveEvenFactors</t>
+  </si>
+  <si>
+    <t>Itération 3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -78,19 +163,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5123,7 +5214,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{D1279524-3F20-E644-915F-D13E0EDCDB7E}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="184" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="184" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5134,7 +5225,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8673830" cy="6282447"/>
+    <xdr:ext cx="8676033" cy="6294783"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Graphique 1">
@@ -5488,26 +5579,25 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="3"/>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B2">
@@ -5542,7 +5632,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="1">
         <v>-3</v>
       </c>
       <c r="B3">
@@ -5587,7 +5677,7 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>-2.9</v>
       </c>
       <c r="B4">
@@ -5632,7 +5722,7 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>-2.8</v>
       </c>
       <c r="B5">
@@ -5677,7 +5767,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>-2.7</v>
       </c>
       <c r="B6">
@@ -5722,7 +5812,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>-2.6</v>
       </c>
       <c r="B7">
@@ -5767,7 +5857,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>-2.5</v>
       </c>
       <c r="B8">
@@ -5812,7 +5902,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>-2.4</v>
       </c>
       <c r="B9">
@@ -5857,7 +5947,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10" s="1">
         <v>-2.2999999999999998</v>
       </c>
       <c r="B10">
@@ -5902,7 +5992,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="A11" s="1">
         <v>-2.2000000000000002</v>
       </c>
       <c r="B11">
@@ -5947,7 +6037,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="A12" s="1">
         <v>-2.1</v>
       </c>
       <c r="B12">
@@ -5992,7 +6082,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="A13" s="1">
         <v>-2</v>
       </c>
       <c r="B13">
@@ -6037,7 +6127,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="A14" s="1">
         <v>-1.9</v>
       </c>
       <c r="B14">
@@ -6082,7 +6172,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="A15" s="1">
         <v>-1.8</v>
       </c>
       <c r="B15">
@@ -6127,7 +6217,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="A16" s="1">
         <v>-1.7</v>
       </c>
       <c r="B16">
@@ -6172,7 +6262,7 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="A17" s="1">
         <v>-1.6</v>
       </c>
       <c r="B17">
@@ -6217,7 +6307,7 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="A18" s="1">
         <v>-1.5</v>
       </c>
       <c r="B18">
@@ -6262,7 +6352,7 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="A19" s="1">
         <v>-1.4</v>
       </c>
       <c r="B19">
@@ -6307,7 +6397,7 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="A20" s="1">
         <v>-1.3</v>
       </c>
       <c r="B20">
@@ -6352,7 +6442,7 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="A21" s="1">
         <v>-1.2</v>
       </c>
       <c r="B21">
@@ -6397,7 +6487,7 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="A22" s="1">
         <v>-1.1000000000000001</v>
       </c>
       <c r="B22">
@@ -6442,7 +6532,7 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="A23" s="1">
         <v>-1</v>
       </c>
       <c r="B23">
@@ -6487,7 +6577,7 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+      <c r="A24" s="1">
         <v>-0.9</v>
       </c>
       <c r="B24">
@@ -6532,7 +6622,7 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+      <c r="A25" s="1">
         <v>-0.8</v>
       </c>
       <c r="B25">
@@ -6577,7 +6667,7 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+      <c r="A26" s="1">
         <v>-0.7</v>
       </c>
       <c r="B26">
@@ -6622,7 +6712,7 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+      <c r="A27" s="1">
         <v>-0.6</v>
       </c>
       <c r="B27">
@@ -6667,7 +6757,7 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+      <c r="A28" s="1">
         <v>-0.5</v>
       </c>
       <c r="B28">
@@ -6712,7 +6802,7 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+      <c r="A29" s="1">
         <v>-0.4</v>
       </c>
       <c r="B29">
@@ -6757,7 +6847,7 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
+      <c r="A30" s="1">
         <v>-0.3</v>
       </c>
       <c r="B30">
@@ -6802,7 +6892,7 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
+      <c r="A31" s="1">
         <v>-0.2</v>
       </c>
       <c r="B31">
@@ -6847,7 +6937,7 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
+      <c r="A32" s="1">
         <v>-0.1</v>
       </c>
       <c r="B32">
@@ -6892,7 +6982,7 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
+      <c r="A33" s="1">
         <v>0</v>
       </c>
       <c r="B33">
@@ -6937,7 +7027,7 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="2">
+      <c r="A34" s="1">
         <v>0.1</v>
       </c>
       <c r="B34">
@@ -6982,7 +7072,7 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
+      <c r="A35" s="1">
         <v>0.2</v>
       </c>
       <c r="B35">
@@ -7027,11 +7117,11 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A36" s="2">
+      <c r="A36" s="1">
         <v>0.3</v>
       </c>
       <c r="B36">
-        <f t="shared" ref="B36:K63" si="2">_xlfn.T.DIST($A36,B$2,FALSE)</f>
+        <f t="shared" ref="B36:K61" si="2">_xlfn.T.DIST($A36,B$2,FALSE)</f>
         <v>0.29202741851723912</v>
       </c>
       <c r="C36">
@@ -7072,7 +7162,7 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A37" s="2">
+      <c r="A37" s="1">
         <v>0.4</v>
       </c>
       <c r="B37">
@@ -7117,7 +7207,7 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
+      <c r="A38" s="1">
         <v>0.5</v>
       </c>
       <c r="B38">
@@ -7162,7 +7252,7 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
+      <c r="A39" s="1">
         <v>0.6</v>
       </c>
       <c r="B39">
@@ -7207,7 +7297,7 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A40" s="2">
+      <c r="A40" s="1">
         <v>0.7</v>
       </c>
       <c r="B40">
@@ -7252,7 +7342,7 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A41" s="2">
+      <c r="A41" s="1">
         <v>0.8</v>
       </c>
       <c r="B41">
@@ -7297,7 +7387,7 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
+      <c r="A42" s="1">
         <v>0.9</v>
       </c>
       <c r="B42">
@@ -7342,7 +7432,7 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A43" s="2">
+      <c r="A43" s="1">
         <v>1</v>
       </c>
       <c r="B43">
@@ -7387,7 +7477,7 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A44" s="2">
+      <c r="A44" s="1">
         <v>1.1000000000000001</v>
       </c>
       <c r="B44">
@@ -7432,7 +7522,7 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A45" s="2">
+      <c r="A45" s="1">
         <v>1.2</v>
       </c>
       <c r="B45">
@@ -7477,7 +7567,7 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="2">
+      <c r="A46" s="1">
         <v>1.3</v>
       </c>
       <c r="B46">
@@ -7522,7 +7612,7 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="2">
+      <c r="A47" s="1">
         <v>1.4</v>
       </c>
       <c r="B47">
@@ -7567,7 +7657,7 @@
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="2">
+      <c r="A48" s="1">
         <v>1.5</v>
       </c>
       <c r="B48">
@@ -7612,7 +7702,7 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A49" s="2">
+      <c r="A49" s="1">
         <v>1.6</v>
       </c>
       <c r="B49">
@@ -7657,7 +7747,7 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A50" s="2">
+      <c r="A50" s="1">
         <v>1.7</v>
       </c>
       <c r="B50">
@@ -7702,7 +7792,7 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A51" s="2">
+      <c r="A51" s="1">
         <v>1.8</v>
       </c>
       <c r="B51">
@@ -7747,7 +7837,7 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" s="2">
+      <c r="A52" s="1">
         <v>1.9</v>
       </c>
       <c r="B52">
@@ -7792,7 +7882,7 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="2">
+      <c r="A53" s="1">
         <v>2</v>
       </c>
       <c r="B53">
@@ -7837,7 +7927,7 @@
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A54" s="2">
+      <c r="A54" s="1">
         <v>2.1</v>
       </c>
       <c r="B54">
@@ -7882,7 +7972,7 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A55" s="2">
+      <c r="A55" s="1">
         <v>2.2000000000000002</v>
       </c>
       <c r="B55">
@@ -7927,7 +8017,7 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A56" s="2">
+      <c r="A56" s="1">
         <v>2.2999999999999998</v>
       </c>
       <c r="B56">
@@ -7972,7 +8062,7 @@
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A57" s="2">
+      <c r="A57" s="1">
         <v>2.4</v>
       </c>
       <c r="B57">
@@ -8017,7 +8107,7 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A58" s="2">
+      <c r="A58" s="1">
         <v>2.5000000000000102</v>
       </c>
       <c r="B58">
@@ -8062,7 +8152,7 @@
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A59" s="2">
+      <c r="A59" s="1">
         <v>2.6</v>
       </c>
       <c r="B59">
@@ -8107,7 +8197,7 @@
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A60" s="2">
+      <c r="A60" s="1">
         <v>2.7</v>
       </c>
       <c r="B60">
@@ -8152,7 +8242,7 @@
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A61" s="2">
+      <c r="A61" s="1">
         <v>2.80000000000001</v>
       </c>
       <c r="B61">
@@ -8197,7 +8287,7 @@
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A62" s="2">
+      <c r="A62" s="1">
         <v>2.9000000000000101</v>
       </c>
       <c r="B62">
@@ -8242,7 +8332,7 @@
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A63" s="2">
+      <c r="A63" s="1">
         <v>3.0000000000000102</v>
       </c>
       <c r="B63">
@@ -8292,4 +8382,744 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D5D7897-C036-1E44-8F4F-F1562C1171B1}">
+  <dimension ref="A1:M20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="3.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+    </row>
+    <row r="2" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3">
+        <v>30</v>
+      </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>30</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>30</v>
+      </c>
+      <c r="L3">
+        <v>8</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>133</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+      <c r="D4">
+        <v>4</v>
+      </c>
+      <c r="E4">
+        <v>133</v>
+      </c>
+      <c r="F4">
+        <v>4</v>
+      </c>
+      <c r="G4">
+        <v>4</v>
+      </c>
+      <c r="H4">
+        <v>133</v>
+      </c>
+      <c r="I4">
+        <v>4</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>127</v>
+      </c>
+      <c r="L4">
+        <v>4</v>
+      </c>
+      <c r="M4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>29</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>29</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>29</v>
+      </c>
+      <c r="I5">
+        <v>3</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5">
+        <v>29</v>
+      </c>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>146</v>
+      </c>
+      <c r="C6">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>146</v>
+      </c>
+      <c r="F6">
+        <v>6</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6">
+        <v>146</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6">
+        <v>146</v>
+      </c>
+      <c r="L6">
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
+        <v>307</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>309</v>
+      </c>
+      <c r="F7">
+        <v>4</v>
+      </c>
+      <c r="G7">
+        <v>3</v>
+      </c>
+      <c r="H7">
+        <v>206</v>
+      </c>
+      <c r="I7">
+        <v>4</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+      <c r="K7">
+        <v>209</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>81</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>81</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>81</v>
+      </c>
+      <c r="I8">
+        <v>3</v>
+      </c>
+      <c r="J8">
+        <v>1</v>
+      </c>
+      <c r="K8">
+        <v>81</v>
+      </c>
+      <c r="L8">
+        <v>3</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>39</v>
+      </c>
+      <c r="C9">
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>39</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>39</v>
+      </c>
+      <c r="I9">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>39</v>
+      </c>
+      <c r="L9">
+        <v>8</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>133</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>133</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>133</v>
+      </c>
+      <c r="I10">
+        <v>3</v>
+      </c>
+      <c r="J10">
+        <v>3</v>
+      </c>
+      <c r="K10">
+        <v>133</v>
+      </c>
+      <c r="L10">
+        <v>3</v>
+      </c>
+      <c r="M10">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>44</v>
+      </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>44</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+      <c r="H11">
+        <v>44</v>
+      </c>
+      <c r="I11">
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>4</v>
+      </c>
+      <c r="K11">
+        <v>44</v>
+      </c>
+      <c r="L11">
+        <v>2</v>
+      </c>
+      <c r="M11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12">
+        <v>24</v>
+      </c>
+      <c r="I12">
+        <v>8</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>24</v>
+      </c>
+      <c r="L12">
+        <v>8</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="H13">
+        <v>22</v>
+      </c>
+      <c r="I13">
+        <v>8</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14">
+        <v>58</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>58</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>58</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>3</v>
+      </c>
+      <c r="K14">
+        <v>58</v>
+      </c>
+      <c r="L14">
+        <v>3</v>
+      </c>
+      <c r="M14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>74</v>
+      </c>
+      <c r="C15">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>4</v>
+      </c>
+      <c r="E15">
+        <v>74</v>
+      </c>
+      <c r="F15">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <v>74</v>
+      </c>
+      <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="J15">
+        <v>4</v>
+      </c>
+      <c r="K15">
+        <v>81</v>
+      </c>
+      <c r="L15">
+        <v>4</v>
+      </c>
+      <c r="M15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>71</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>72</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>4</v>
+      </c>
+      <c r="E17">
+        <v>72</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>72</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>86</v>
+      </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>86</v>
+      </c>
+      <c r="F18">
+        <v>4</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>86</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>84</v>
+      </c>
+      <c r="L18">
+        <v>5</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="3">
+        <f>SUM(B3:B18)</f>
+        <v>1303</v>
+      </c>
+      <c r="C19" s="3">
+        <f t="shared" ref="C19:D19" si="0">SUM(C3:C18)</f>
+        <v>60</v>
+      </c>
+      <c r="D19" s="3">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="E19" s="3">
+        <f>SUM(E3:E18)</f>
+        <v>1234</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" ref="F19" si="1">SUM(F3:F18)</f>
+        <v>56</v>
+      </c>
+      <c r="G19" s="3">
+        <f t="shared" ref="G19" si="2">SUM(G3:G18)</f>
+        <v>31</v>
+      </c>
+      <c r="H19" s="3">
+        <f>SUM(H3:H18)</f>
+        <v>1177</v>
+      </c>
+      <c r="I19" s="3">
+        <f t="shared" ref="I19" si="3">SUM(I3:I18)</f>
+        <v>72</v>
+      </c>
+      <c r="J19" s="3">
+        <f t="shared" ref="J19" si="4">SUM(J3:J18)</f>
+        <v>31</v>
+      </c>
+      <c r="K19" s="3">
+        <f>SUM(K3:K18)</f>
+        <v>1085</v>
+      </c>
+      <c r="L19" s="3">
+        <f t="shared" ref="L19" si="5">SUM(L3:L18)</f>
+        <v>61</v>
+      </c>
+      <c r="M19" s="3">
+        <f t="shared" ref="M19" si="6">SUM(M3:M18)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E20" s="5">
+        <f>(E19-$B19)/$B19</f>
+        <v>-5.2954719877206444E-2</v>
+      </c>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5">
+        <f t="shared" ref="F20:J20" si="7">(H19-$B19)/$B19</f>
+        <v>-9.6699923254029166E-2</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5">
+        <f t="shared" ref="K20" si="8">(K19-$B19)/$B19</f>
+        <v>-0.16730621642363777</v>
+      </c>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="E1:G1"/>
+    <mergeCell ref="H1:J1"/>
+    <mergeCell ref="K1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>